<commit_message>
Actualización del cronograma 24/06
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/documentos/SCIP-CP.xlsx
+++ b/2-Desarrollo/SCIP/documentos/SCIP-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing. de Software\8 - Gestión de Configuración y Mantenimiento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434936A1-BCE1-439E-ACB1-AB6A757D0203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AB4195-E281-4201-B6B0-A7073EC7C41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B688ADBF-7033-4F25-B77C-86C1BC07C039}"/>
   </bookViews>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3B3B80-6AC9-4507-B19B-F46B6EBD1C86}">
   <dimension ref="B1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3226,7 +3226,7 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="20">
-        <v>0.41</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="M45" s="21" t="s">
         <v>12</v>
@@ -3334,7 +3334,7 @@
         <v>223</v>
       </c>
       <c r="L48" s="9">
-        <v>0.05</v>
+        <v>0.8</v>
       </c>
       <c r="M48" s="13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Actualización del Cronograma 28/06
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/documentos/SCIP-CP.xlsx
+++ b/2-Desarrollo/SCIP/documentos/SCIP-CP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing. de Software\8 - Gestión de Configuración y Mantenimiento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing. de Software\8 - Gestión de Configuración y Mantenimiento\Proyecto G4\Softgenix-Peru\2-Desarrollo\SCIP\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AB4195-E281-4201-B6B0-A7073EC7C41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5518C75-8931-4504-9CED-B5A43A564754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B688ADBF-7033-4F25-B77C-86C1BC07C039}"/>
   </bookViews>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3B3B80-6AC9-4507-B19B-F46B6EBD1C86}">
   <dimension ref="B1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3226,7 +3226,7 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="20">
-        <v>0.56000000000000005</v>
+        <v>0.65</v>
       </c>
       <c r="M45" s="21" t="s">
         <v>12</v>
@@ -3334,7 +3334,7 @@
         <v>223</v>
       </c>
       <c r="L48" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="M48" s="13" t="s">
         <v>12</v>
@@ -3370,7 +3370,7 @@
         <v>205</v>
       </c>
       <c r="L49" s="9">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="M49" s="13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Actualización de cronograma del proyecto
</commit_message>
<xml_diff>
--- a/2-Desarrollo/SCIP/documentos/SCIP-CP.xlsx
+++ b/2-Desarrollo/SCIP/documentos/SCIP-CP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing. de Software\8 - Gestión de Configuración y Mantenimiento\Proyecto G4\Softgenix-Peru\2-Desarrollo\SCIP\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAFE4B1-B8CF-48F0-9BF9-4F44A40EF8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACED879-8977-47B1-B9EB-C31BA3F290E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="1020" windowWidth="19410" windowHeight="11295" xr2:uid="{B688ADBF-7033-4F25-B77C-86C1BC07C039}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B688ADBF-7033-4F25-B77C-86C1BC07C039}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3B3B80-6AC9-4507-B19B-F46B6EBD1C86}">
   <dimension ref="B1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P44" sqref="P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3226,7 +3226,7 @@
       <c r="J45" s="19"/>
       <c r="K45" s="19"/>
       <c r="L45" s="20">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="M45" s="21" t="s">
         <v>12</v>
@@ -3406,7 +3406,7 @@
         <v>127</v>
       </c>
       <c r="L50" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M50" s="27" t="s">
         <v>48</v>

</xml_diff>